<commit_message>
Updated requiremens in manula tests spreadsheet
</commit_message>
<xml_diff>
--- a/Manul Test Steps/Manual Tests EE Booking form.xlsx
+++ b/Manul Test Steps/Manual Tests EE Booking form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ravi/Documents/GitHub/rav-test-ee/Manul Test Steps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE2EE3C-8388-D54A-9F46-A835540AD804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03556CA-B06A-0A4A-A163-96C20827761A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creating a booking" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
   <si>
     <t xml:space="preserve">Test step Aim </t>
-  </si>
-  <si>
-    <t>Objective</t>
   </si>
   <si>
     <t>Description</t>
@@ -354,9 +351,6 @@
      3. Save booking and check result ( Result A)</t>
   </si>
   <si>
-    <t>To Check if a booking can be saved with invalid values</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test Aim </t>
   </si>
   <si>
@@ -370,6 +364,15 @@
   </si>
   <si>
     <t>An internet connection and browsers are required to run the tests</t>
+  </si>
+  <si>
+    <t>Additonal requirement</t>
+  </si>
+  <si>
+    <t>To check if a booking can be deleted</t>
+  </si>
+  <si>
+    <t>To check if a booking can be saved with invalid values</t>
   </si>
 </sst>
 </file>
@@ -743,8 +746,8 @@
   </sheetPr>
   <dimension ref="A1:I1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -762,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="2"/>
@@ -774,10 +777,10 @@
     <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
@@ -789,10 +792,10 @@
     <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2"/>
@@ -804,10 +807,10 @@
     <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
@@ -828,28 +831,28 @@
     </row>
     <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="56" x14ac:dyDescent="0.15">
@@ -857,25 +860,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
@@ -883,25 +886,25 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="140" x14ac:dyDescent="0.15">
@@ -909,25 +912,25 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="F9" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="140" x14ac:dyDescent="0.15">
@@ -935,25 +938,25 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="70" x14ac:dyDescent="0.15">
@@ -961,25 +964,25 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="70" x14ac:dyDescent="0.15">
@@ -987,25 +990,25 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="70" x14ac:dyDescent="0.15">
@@ -1013,25 +1016,25 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -10948,8 +10951,8 @@
   </sheetPr>
   <dimension ref="B1:J1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10965,10 +10968,10 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="2"/>
@@ -10980,10 +10983,10 @@
     </row>
     <row r="2" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="2"/>
@@ -10995,10 +10998,10 @@
     </row>
     <row r="3" spans="2:10" ht="154" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="2"/>
@@ -11010,10 +11013,10 @@
     </row>
     <row r="4" spans="2:10" ht="28" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="2"/>
@@ -11036,31 +11039,31 @@
     </row>
     <row r="6" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B6" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="42" x14ac:dyDescent="0.15">
@@ -11068,25 +11071,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="J7" s="16"/>
     </row>
@@ -11095,25 +11098,25 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
+      <c r="F8" s="17" t="s">
+        <v>23</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="J8" s="16"/>
     </row>
@@ -11122,16 +11125,16 @@
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F9" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -11143,28 +11146,28 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>44</v>
+      <c r="F10" s="17" t="s">
+        <v>23</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="J10" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="182" x14ac:dyDescent="0.15">
@@ -11172,28 +11175,28 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="J11" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="345" x14ac:dyDescent="0.15">
@@ -11201,25 +11204,25 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="J12" s="16"/>
     </row>
@@ -11228,28 +11231,28 @@
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="J13" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="126" x14ac:dyDescent="0.15">
@@ -11257,28 +11260,28 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>61</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="J14" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.15">
@@ -22162,6 +22165,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -22173,7 +22177,7 @@
   <dimension ref="B1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -22187,9 +22191,11 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="D1" s="15"/>
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
@@ -22199,10 +22205,10 @@
     </row>
     <row r="2" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="3"/>
@@ -22213,10 +22219,10 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="3"/>
@@ -22227,10 +22233,10 @@
     </row>
     <row r="4" spans="2:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="3"/>
@@ -22251,28 +22257,28 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="168" x14ac:dyDescent="0.15">
@@ -22280,25 +22286,25 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="168" x14ac:dyDescent="0.15">
@@ -22306,25 +22312,25 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.15">

</xml_diff>